<commit_message>
Dec 21 5:04 PM
</commit_message>
<xml_diff>
--- a/assets/public/user_upload/candidates_partten.xlsx
+++ b/assets/public/user_upload/candidates_partten.xlsx
@@ -25,13 +25,13 @@
     <t xml:space="preserve">username</t>
   </si>
   <si>
-    <t xml:space="preserve">quandh28</t>
+    <t xml:space="preserve">quandohong28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zthanh13</t>
   </si>
   <si>
     <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zthanh13</t>
   </si>
 </sst>
 </file>
@@ -136,7 +136,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>